<commit_message>
dejo sin base_vat ni base_iban
</commit_message>
<xml_diff>
--- a/l10n_ec_chart/data/account.account.template.xlsx
+++ b/l10n_ec_chart/data/account.account.template.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2857" uniqueCount="623">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2858" uniqueCount="624">
   <si>
     <t>id</t>
   </si>
@@ -1889,6 +1889,9 @@
   </si>
   <si>
     <t>nocreate</t>
+  </si>
+  <si>
+    <t>520305</t>
   </si>
 </sst>
 </file>
@@ -2789,18 +2792,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G501"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C484" sqref="C484"/>
+    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
+      <selection activeCell="A57" sqref="A57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.5703125" style="15" customWidth="1"/>
-    <col min="2" max="3" width="11.42578125" style="8"/>
+    <col min="1" max="1" width="12.85546875" style="15" customWidth="1"/>
+    <col min="2" max="3" width="9.42578125" style="8" customWidth="1"/>
     <col min="4" max="4" width="13.28515625" style="15" customWidth="1"/>
-    <col min="5" max="5" width="72" style="8" customWidth="1"/>
-    <col min="6" max="6" width="46.7109375" style="8" customWidth="1"/>
-    <col min="7" max="7" width="21.28515625" style="8" customWidth="1"/>
+    <col min="5" max="5" width="81.140625" style="8" customWidth="1"/>
+    <col min="6" max="6" width="39.140625" style="8" customWidth="1"/>
+    <col min="7" max="7" width="18.28515625" style="8" customWidth="1"/>
     <col min="8" max="16384" width="11.42578125" style="8"/>
   </cols>
   <sheetData>
@@ -4675,7 +4678,7 @@
         <v>6</v>
       </c>
       <c r="C82" s="10" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="D82" s="14">
         <v>1010801</v>
@@ -4698,7 +4701,7 @@
         <v>6</v>
       </c>
       <c r="C83" s="10" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="D83" s="14">
         <v>101080101</v>
@@ -6262,7 +6265,7 @@
         <v>18</v>
       </c>
       <c r="C151" s="8" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="D151" s="15">
         <v>2010301</v>
@@ -6285,7 +6288,7 @@
         <v>18</v>
       </c>
       <c r="C152" s="8" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="D152" s="15">
         <v>2010302</v>
@@ -6515,7 +6518,7 @@
         <v>6</v>
       </c>
       <c r="C162" s="10" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="D162" s="14" t="s">
         <v>318</v>
@@ -6722,7 +6725,7 @@
         <v>6</v>
       </c>
       <c r="C171" s="10" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="D171" s="14" t="s">
         <v>338</v>
@@ -7136,7 +7139,7 @@
         <v>6</v>
       </c>
       <c r="C189" s="10" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="D189" s="14" t="s">
         <v>340</v>
@@ -11414,7 +11417,7 @@
         <v>6</v>
       </c>
       <c r="C375" s="10" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="D375" s="14" t="s">
         <v>505</v>
@@ -12725,7 +12728,7 @@
         <v>6</v>
       </c>
       <c r="C432" s="10" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="D432" s="14" t="s">
         <v>543</v>
@@ -13845,8 +13848,8 @@
       </c>
     </row>
     <row r="481" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A481" s="15">
-        <v>520305</v>
+      <c r="A481" s="15" t="s">
+        <v>623</v>
       </c>
       <c r="B481" s="8" t="s">
         <v>6</v>

</xml_diff>